<commit_message>
Changed symbol properties for cleaner BOM generation
</commit_message>
<xml_diff>
--- a/Card/L1IFStream.xlsx
+++ b/Card/L1IFStream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\GPS\L1IFStream\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA0AC0B-787A-4828-BDDE-A30B2BB076CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A834EE0D-2E5D-41D2-9D6A-70C36FD2E242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7930" yWindow="1850" windowWidth="21550" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="530" yWindow="3720" windowWidth="25020" windowHeight="16970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1IFStream" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="299">
   <si>
     <t>Source:</t>
   </si>
@@ -535,9 +535,6 @@
     <t>MAX2769BETI/V+</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>TPS717285DCKR</t>
   </si>
   <si>
@@ -553,12 +550,6 @@
     <t>296-19649-1-ND</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>L1IFStream-rescue:TPS717285DCKR-MAX2769FT2232H</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -682,9 +673,6 @@
     <t>U11</t>
   </si>
   <si>
-    <t>74HC2G04</t>
-  </si>
-  <si>
     <t>:74HC2G04-MAX2769FT2232H_2</t>
   </si>
   <si>
@@ -697,9 +685,6 @@
     <t>IC INVERTER 2CH 2-INP 6TSSOP</t>
   </si>
   <si>
-    <t>1727-6045-1-ND</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -769,15 +754,9 @@
     <t>330 Ohms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200, Moisture Resistant Thick Film</t>
   </si>
   <si>
-    <t>Distributor</t>
-  </si>
-  <si>
     <t>DigiKey</t>
   </si>
   <si>
-    <t>Distributor P/N#</t>
-  </si>
-  <si>
     <t>MFR</t>
   </si>
   <si>
@@ -904,9 +883,6 @@
     <t>74LVC374APW,118</t>
   </si>
   <si>
-    <t>74HC2G04GW,125</t>
-  </si>
-  <si>
     <t>SiTime</t>
   </si>
   <si>
@@ -917,6 +893,30 @@
   </si>
   <si>
     <t>QPQ1060SR</t>
+  </si>
+  <si>
+    <t>74HC2GU04GW,125</t>
+  </si>
+  <si>
+    <t>74HC2GU04</t>
+  </si>
+  <si>
+    <t>1727-6915-6-ND</t>
+  </si>
+  <si>
+    <t>Signal Conditioning L1 TC-SAW, GSO</t>
+  </si>
+  <si>
+    <t>MEMS OSC TCXO 16.3680MHZ</t>
+  </si>
+  <si>
+    <t>U2, U3</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Vendor P/N#</t>
   </si>
 </sst>
 </file>
@@ -1400,9 +1400,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1758,15 +1759,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
     <col min="4" max="4" width="21.6328125" customWidth="1"/>
     <col min="5" max="6" width="16.54296875" customWidth="1"/>
     <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
@@ -1776,7 +1778,7 @@
     <col min="11" max="11" width="45" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="27.453125" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="66.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="66.7265625" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1842,19 +1844,19 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>249</v>
+        <v>297</v>
       </c>
       <c r="I9" t="s">
-        <v>251</v>
+        <v>298</v>
       </c>
       <c r="J9" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -1892,13 +1894,13 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G10" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I10" t="s">
         <v>27</v>
@@ -1927,13 +1929,13 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G11" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -1962,13 +1964,13 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G12" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H12" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I12" t="s">
         <v>35</v>
@@ -1997,13 +1999,13 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="G13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H13" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I13" t="s">
         <v>39</v>
@@ -2032,19 +2034,19 @@
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G14" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H14" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I14" t="s">
         <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -2070,13 +2072,13 @@
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="G15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I15" t="s">
         <v>45</v>
@@ -2105,13 +2107,13 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G16" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="H16" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I16" t="s">
         <v>49</v>
@@ -2140,13 +2142,13 @@
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="G17" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H17" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I17" t="s">
         <v>54</v>
@@ -2175,13 +2177,13 @@
         <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G18" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H18" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I18" t="s">
         <v>58</v>
@@ -2207,13 +2209,13 @@
         <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I19" t="s">
         <v>64</v>
@@ -2245,13 +2247,13 @@
         <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G20" t="s">
         <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I20" t="s">
         <v>72</v>
@@ -2286,13 +2288,13 @@
         <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G21" t="s">
         <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I21" t="s">
         <v>80</v>
@@ -2324,13 +2326,13 @@
         <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G22" t="s">
         <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I22" t="s">
         <v>88</v>
@@ -2365,13 +2367,13 @@
         <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G23" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H23" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I23" t="s">
         <v>94</v>
@@ -2397,10 +2399,10 @@
         <v>96</v>
       </c>
       <c r="F24" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H24" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="K24" t="s">
         <v>97</v>
@@ -2426,13 +2428,13 @@
         <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="G25">
         <v>132136</v>
       </c>
       <c r="H25" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I25" t="s">
         <v>105</v>
@@ -2464,13 +2466,13 @@
         <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G26">
         <v>480372200</v>
       </c>
       <c r="H26" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I26" t="s">
         <v>111</v>
@@ -2502,13 +2504,13 @@
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="G27" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H27" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I27" t="s">
         <v>117</v>
@@ -2537,13 +2539,13 @@
         <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="G28" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H28" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I28" t="s">
         <v>121</v>
@@ -2575,13 +2577,13 @@
         <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G29" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H29" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I29" t="s">
         <v>127</v>
@@ -2610,13 +2612,13 @@
         <v>129</v>
       </c>
       <c r="F30" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G30" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H30" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
@@ -2645,19 +2647,19 @@
         <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G31" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H31" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
       </c>
       <c r="J31" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K31" t="s">
         <v>130</v>
@@ -2683,13 +2685,13 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G32" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H32" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I32" t="s">
         <v>136</v>
@@ -2718,13 +2720,13 @@
         <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G33" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I33" t="s">
         <v>141</v>
@@ -2753,13 +2755,13 @@
         <v>143</v>
       </c>
       <c r="F34" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G34" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H34" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I34" t="s">
         <v>147</v>
@@ -2791,13 +2793,13 @@
         <v>149</v>
       </c>
       <c r="F35" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G35" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H35" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I35" t="s">
         <v>151</v>
@@ -2826,13 +2828,13 @@
         <v>153</v>
       </c>
       <c r="F36" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G36" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="H36" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I36" t="s">
         <v>155</v>
@@ -2861,13 +2863,13 @@
         <v>143</v>
       </c>
       <c r="F37" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G37" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H37" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I37" t="s">
         <v>147</v>
@@ -2884,7 +2886,7 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2896,16 +2898,16 @@
         <v>330</v>
       </c>
       <c r="F38" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G38" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H38" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I38" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K38" t="s">
         <v>130</v>
@@ -2914,7 +2916,7 @@
         <v>131</v>
       </c>
       <c r="O38" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
@@ -2931,10 +2933,10 @@
         <v>159</v>
       </c>
       <c r="F39" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H39" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="K39" t="s">
         <v>160</v>
@@ -2963,13 +2965,13 @@
         <v>163</v>
       </c>
       <c r="F40" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="G40" t="s">
         <v>170</v>
       </c>
       <c r="H40" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I40" t="s">
         <v>169</v>
@@ -2992,34 +2994,34 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>296</v>
+      </c>
+      <c r="E41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" t="s">
+        <v>260</v>
+      </c>
+      <c r="G41" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I41" t="s">
         <v>175</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>171</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="K41" t="s">
         <v>172</v>
       </c>
-      <c r="F41" t="s">
-        <v>267</v>
-      </c>
-      <c r="G41" t="s">
-        <v>172</v>
-      </c>
-      <c r="H41" t="s">
-        <v>250</v>
-      </c>
-      <c r="I41" t="s">
-        <v>176</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>173</v>
-      </c>
-      <c r="L41" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -3027,34 +3029,37 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" t="s">
         <v>177</v>
       </c>
-      <c r="E42" t="s">
-        <v>172</v>
-      </c>
       <c r="F42" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="H42" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="K42" t="s">
         <v>178</v>
       </c>
       <c r="L42" t="s">
-        <v>174</v>
+        <v>179</v>
+      </c>
+      <c r="M42" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
@@ -3062,37 +3067,34 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E43" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F43" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G43" t="s">
-        <v>180</v>
+        <v>279</v>
       </c>
       <c r="H43" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I43" t="s">
+        <v>188</v>
+      </c>
+      <c r="K43" t="s">
         <v>185</v>
       </c>
-      <c r="K43" t="s">
-        <v>181</v>
-      </c>
       <c r="L43" t="s">
-        <v>182</v>
-      </c>
-      <c r="M43" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
@@ -3100,34 +3102,34 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F44" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G44" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="H44" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I44" t="s">
+        <v>194</v>
+      </c>
+      <c r="K44" t="s">
         <v>191</v>
       </c>
-      <c r="K44" t="s">
-        <v>188</v>
-      </c>
       <c r="L44" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
@@ -3135,34 +3137,37 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E45" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F45" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G45" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H45" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I45" t="s">
+        <v>201</v>
+      </c>
+      <c r="K45" t="s">
         <v>197</v>
       </c>
-      <c r="K45" t="s">
-        <v>194</v>
-      </c>
       <c r="L45" t="s">
-        <v>195</v>
+        <v>198</v>
+      </c>
+      <c r="M45" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -3170,37 +3175,37 @@
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E46" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F46" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G46" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H46" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I46" t="s">
+        <v>208</v>
+      </c>
+      <c r="K46" t="s">
         <v>204</v>
       </c>
-      <c r="K46" t="s">
-        <v>200</v>
-      </c>
       <c r="L46" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="M46" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
@@ -3208,37 +3213,37 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>209</v>
+      </c>
+      <c r="E47" t="s">
         <v>210</v>
       </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>205</v>
-      </c>
-      <c r="E47" t="s">
-        <v>206</v>
-      </c>
       <c r="F47" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G47" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H47" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I47" t="s">
+        <v>215</v>
+      </c>
+      <c r="K47" t="s">
         <v>211</v>
       </c>
-      <c r="K47" t="s">
-        <v>207</v>
-      </c>
       <c r="L47" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="M47" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
@@ -3246,37 +3251,37 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
+        <v>220</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F48" t="s">
+        <v>284</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H48" t="s">
+        <v>244</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K48" t="s">
         <v>217</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
-        <v>212</v>
-      </c>
-      <c r="E48" t="s">
-        <v>213</v>
-      </c>
-      <c r="F48" t="s">
-        <v>291</v>
-      </c>
-      <c r="G48" t="s">
-        <v>293</v>
-      </c>
-      <c r="H48" t="s">
-        <v>250</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="L48" t="s">
         <v>218</v>
       </c>
-      <c r="K48" t="s">
-        <v>214</v>
-      </c>
-      <c r="L48" t="s">
-        <v>215</v>
-      </c>
       <c r="M48" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
@@ -3284,74 +3289,74 @@
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>295</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E49" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F49" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G49" t="s">
-        <v>294</v>
+        <v>228</v>
       </c>
       <c r="H49" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I49" t="s">
+        <v>226</v>
+      </c>
+      <c r="K49" t="s">
+        <v>223</v>
+      </c>
+      <c r="L49" t="s">
+        <v>224</v>
+      </c>
+      <c r="M49" t="s">
         <v>225</v>
       </c>
-      <c r="K49" t="s">
-        <v>221</v>
-      </c>
-      <c r="L49" t="s">
-        <v>222</v>
-      </c>
-      <c r="M49" t="s">
-        <v>223</v>
+      <c r="P49" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>41</v>
       </c>
+      <c r="B50" t="s">
+        <v>233</v>
+      </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F50" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G50" t="s">
-        <v>233</v>
+        <v>288</v>
       </c>
       <c r="H50" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I50" t="s">
+        <v>234</v>
+      </c>
+      <c r="K50" t="s">
         <v>231</v>
       </c>
-      <c r="K50" t="s">
-        <v>228</v>
-      </c>
       <c r="L50" t="s">
-        <v>229</v>
-      </c>
-      <c r="M50" t="s">
-        <v>230</v>
-      </c>
-      <c r="P50" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3360,69 +3365,37 @@
         <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E51" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F51" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G51" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="H51" t="s">
-        <v>250</v>
+        <v>21</v>
       </c>
       <c r="I51" t="s">
+        <v>240</v>
+      </c>
+      <c r="K51" t="s">
+        <v>237</v>
+      </c>
+      <c r="L51" t="s">
+        <v>238</v>
+      </c>
+      <c r="M51" t="s">
         <v>239</v>
-      </c>
-      <c r="K51" t="s">
-        <v>236</v>
-      </c>
-      <c r="L51" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>43</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>240</v>
-      </c>
-      <c r="E52" t="s">
-        <v>241</v>
-      </c>
-      <c r="F52" t="s">
-        <v>297</v>
-      </c>
-      <c r="G52" t="s">
-        <v>298</v>
-      </c>
-      <c r="H52" t="s">
-        <v>21</v>
-      </c>
-      <c r="I52" t="s">
-        <v>245</v>
-      </c>
-      <c r="K52" t="s">
-        <v>242</v>
-      </c>
-      <c r="L52" t="s">
-        <v>243</v>
-      </c>
-      <c r="M52" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
U11 should be unbuffered inverter. Should it be non-inverting?
</commit_message>
<xml_diff>
--- a/Card/L1IFStream.xlsx
+++ b/Card/L1IFStream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\GPS\L1IFStream\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A834EE0D-2E5D-41D2-9D6A-70C36FD2E242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6211C31E-6C13-450C-867E-B0C9F12D5462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="3720" windowWidth="25020" windowHeight="16970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="3790" windowWidth="25020" windowHeight="16970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1IFStream" sheetId="1" r:id="rId1"/>
@@ -424,18 +424,12 @@
     <t>2019-RK73H1JTTD2002FCT-ND</t>
   </si>
   <si>
-    <t>R2, R4, R5, R6, R7</t>
-  </si>
-  <si>
     <t>RES 0 OHM JUMPER 0603</t>
   </si>
   <si>
     <t>2019-RK73Z1JTTDCT-ND</t>
   </si>
   <si>
-    <t>R3, R8, R9, R10, R11</t>
-  </si>
-  <si>
     <t>R12</t>
   </si>
   <si>
@@ -917,13 +911,19 @@
   </si>
   <si>
     <t>Vendor P/N#</t>
+  </si>
+  <si>
+    <t>R3, R6, R8, R9, R10</t>
+  </si>
+  <si>
+    <t>R2, R4, R5, R7, R11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1054,6 +1054,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1403,7 +1409,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1761,14 +1767,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="21.6328125" customWidth="1"/>
     <col min="5" max="6" width="16.54296875" customWidth="1"/>
     <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
@@ -1844,19 +1850,19 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -1894,13 +1900,13 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I10" t="s">
         <v>27</v>
@@ -1929,13 +1935,13 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G11" t="s">
         <v>247</v>
       </c>
-      <c r="G11" t="s">
-        <v>249</v>
-      </c>
       <c r="H11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
@@ -1964,13 +1970,13 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I12" t="s">
         <v>35</v>
@@ -1999,13 +2005,13 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I13" t="s">
         <v>39</v>
@@ -2034,19 +2040,19 @@
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H14" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>251</v>
       </c>
       <c r="J14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -2072,13 +2078,13 @@
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I15" t="s">
         <v>45</v>
@@ -2107,13 +2113,13 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I16" t="s">
         <v>49</v>
@@ -2142,13 +2148,13 @@
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I17" t="s">
         <v>54</v>
@@ -2177,13 +2183,13 @@
         <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I18" t="s">
         <v>58</v>
@@ -2209,13 +2215,13 @@
         <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I19" t="s">
         <v>64</v>
@@ -2247,13 +2253,13 @@
         <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G20" t="s">
         <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I20" t="s">
         <v>72</v>
@@ -2288,13 +2294,13 @@
         <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G21" t="s">
         <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I21" t="s">
         <v>80</v>
@@ -2326,13 +2332,13 @@
         <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G22" t="s">
         <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I22" t="s">
         <v>88</v>
@@ -2367,13 +2373,13 @@
         <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I23" t="s">
         <v>94</v>
@@ -2399,10 +2405,10 @@
         <v>96</v>
       </c>
       <c r="F24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K24" t="s">
         <v>97</v>
@@ -2428,13 +2434,13 @@
         <v>100</v>
       </c>
       <c r="F25" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G25">
         <v>132136</v>
       </c>
       <c r="H25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I25" t="s">
         <v>105</v>
@@ -2466,13 +2472,13 @@
         <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G26">
         <v>480372200</v>
       </c>
       <c r="H26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I26" t="s">
         <v>111</v>
@@ -2504,13 +2510,13 @@
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I27" t="s">
         <v>117</v>
@@ -2539,13 +2545,13 @@
         <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H28" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I28" t="s">
         <v>121</v>
@@ -2577,13 +2583,13 @@
         <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H29" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I29" t="s">
         <v>127</v>
@@ -2612,13 +2618,13 @@
         <v>129</v>
       </c>
       <c r="F30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H30" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
@@ -2635,31 +2641,28 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C31">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" t="s">
-        <v>41</v>
+        <v>298</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="G31" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="H31" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I31" t="s">
-        <v>136</v>
-      </c>
-      <c r="J31" t="s">
-        <v>253</v>
+        <v>135</v>
       </c>
       <c r="K31" t="s">
         <v>130</v>
@@ -2673,28 +2676,31 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
+        <v>297</v>
+      </c>
+      <c r="E32" t="s">
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="G32" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="H32" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="I32" t="s">
-        <v>136</v>
+        <v>251</v>
+      </c>
+      <c r="J32" t="s">
+        <v>251</v>
       </c>
       <c r="K32" t="s">
         <v>130</v>
@@ -2708,28 +2714,28 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E33" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>268</v>
+      </c>
+      <c r="G33" t="s">
+        <v>270</v>
+      </c>
+      <c r="H33" t="s">
+        <v>242</v>
+      </c>
+      <c r="I33" t="s">
         <v>139</v>
-      </c>
-      <c r="F33" t="s">
-        <v>270</v>
-      </c>
-      <c r="G33" t="s">
-        <v>272</v>
-      </c>
-      <c r="H33" t="s">
-        <v>244</v>
-      </c>
-      <c r="I33" t="s">
-        <v>141</v>
       </c>
       <c r="K33" t="s">
         <v>130</v>
@@ -2743,37 +2749,37 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" t="s">
+        <v>271</v>
+      </c>
+      <c r="H34" t="s">
+        <v>242</v>
+      </c>
+      <c r="I34" t="s">
+        <v>145</v>
+      </c>
+      <c r="K34" t="s">
         <v>142</v>
-      </c>
-      <c r="E34" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" t="s">
-        <v>270</v>
-      </c>
-      <c r="G34" t="s">
-        <v>273</v>
-      </c>
-      <c r="H34" t="s">
-        <v>244</v>
-      </c>
-      <c r="I34" t="s">
-        <v>147</v>
-      </c>
-      <c r="K34" t="s">
-        <v>144</v>
       </c>
       <c r="L34" t="s">
         <v>131</v>
       </c>
       <c r="M34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
@@ -2781,28 +2787,28 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" t="s">
+        <v>268</v>
+      </c>
+      <c r="G35" t="s">
+        <v>272</v>
+      </c>
+      <c r="H35" t="s">
+        <v>242</v>
+      </c>
+      <c r="I35" t="s">
         <v>149</v>
-      </c>
-      <c r="F35" t="s">
-        <v>270</v>
-      </c>
-      <c r="G35" t="s">
-        <v>274</v>
-      </c>
-      <c r="H35" t="s">
-        <v>244</v>
-      </c>
-      <c r="I35" t="s">
-        <v>151</v>
       </c>
       <c r="K35" t="s">
         <v>130</v>
@@ -2816,28 +2822,28 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" t="s">
+        <v>268</v>
+      </c>
+      <c r="G36" t="s">
+        <v>273</v>
+      </c>
+      <c r="H36" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" t="s">
         <v>153</v>
-      </c>
-      <c r="F36" t="s">
-        <v>270</v>
-      </c>
-      <c r="G36" t="s">
-        <v>275</v>
-      </c>
-      <c r="H36" t="s">
-        <v>244</v>
-      </c>
-      <c r="I36" t="s">
-        <v>155</v>
       </c>
       <c r="K36" t="s">
         <v>130</v>
@@ -2851,28 +2857,28 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K37" t="s">
         <v>130</v>
@@ -2886,28 +2892,28 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E38">
         <v>330</v>
       </c>
       <c r="F38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G38" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K38" t="s">
         <v>130</v>
@@ -2916,7 +2922,7 @@
         <v>131</v>
       </c>
       <c r="O38" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
@@ -2927,25 +2933,25 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" t="s">
+        <v>260</v>
+      </c>
+      <c r="H39" t="s">
+        <v>243</v>
+      </c>
+      <c r="K39" t="s">
         <v>158</v>
       </c>
-      <c r="E39" t="s">
+      <c r="L39" t="s">
         <v>159</v>
       </c>
-      <c r="F39" t="s">
-        <v>262</v>
-      </c>
-      <c r="H39" t="s">
-        <v>245</v>
-      </c>
-      <c r="K39" t="s">
-        <v>160</v>
-      </c>
-      <c r="L39" t="s">
-        <v>161</v>
-      </c>
       <c r="M39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
@@ -2953,40 +2959,40 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" t="s">
+        <v>275</v>
+      </c>
+      <c r="G40" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" t="s">
+        <v>242</v>
+      </c>
+      <c r="I40" t="s">
+        <v>167</v>
+      </c>
+      <c r="K40" t="s">
         <v>162</v>
       </c>
-      <c r="E40" t="s">
+      <c r="L40" t="s">
         <v>163</v>
       </c>
-      <c r="F40" t="s">
-        <v>277</v>
-      </c>
-      <c r="G40" t="s">
-        <v>170</v>
-      </c>
-      <c r="H40" t="s">
-        <v>244</v>
-      </c>
-      <c r="I40" t="s">
-        <v>169</v>
-      </c>
-      <c r="K40" t="s">
+      <c r="M40" t="s">
         <v>164</v>
       </c>
-      <c r="L40" t="s">
-        <v>165</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="O40" t="s">
         <v>166</v>
-      </c>
-      <c r="O40" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
@@ -2994,34 +3000,34 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E41" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" t="s">
+        <v>258</v>
+      </c>
+      <c r="G41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H41" t="s">
+        <v>242</v>
+      </c>
+      <c r="I41" t="s">
+        <v>173</v>
+      </c>
+      <c r="K41" t="s">
+        <v>170</v>
+      </c>
+      <c r="L41" t="s">
         <v>171</v>
-      </c>
-      <c r="F41" t="s">
-        <v>260</v>
-      </c>
-      <c r="G41" t="s">
-        <v>171</v>
-      </c>
-      <c r="H41" t="s">
-        <v>244</v>
-      </c>
-      <c r="I41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K41" t="s">
-        <v>172</v>
-      </c>
-      <c r="L41" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -3029,37 +3035,37 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" t="s">
+        <v>276</v>
+      </c>
+      <c r="G42" t="s">
+        <v>175</v>
+      </c>
+      <c r="H42" t="s">
+        <v>242</v>
+      </c>
+      <c r="I42" t="s">
+        <v>180</v>
+      </c>
+      <c r="K42" t="s">
         <v>176</v>
       </c>
-      <c r="E42" t="s">
+      <c r="L42" t="s">
         <v>177</v>
       </c>
-      <c r="F42" t="s">
-        <v>278</v>
-      </c>
-      <c r="G42" t="s">
-        <v>177</v>
-      </c>
-      <c r="H42" t="s">
-        <v>244</v>
-      </c>
-      <c r="I42" t="s">
-        <v>182</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="M42" t="s">
         <v>178</v>
-      </c>
-      <c r="L42" t="s">
-        <v>179</v>
-      </c>
-      <c r="M42" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
@@ -3067,34 +3073,34 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" t="s">
+        <v>277</v>
+      </c>
+      <c r="H43" t="s">
+        <v>242</v>
+      </c>
+      <c r="I43" t="s">
+        <v>186</v>
+      </c>
+      <c r="K43" t="s">
         <v>183</v>
       </c>
-      <c r="E43" t="s">
+      <c r="L43" t="s">
         <v>184</v>
-      </c>
-      <c r="F43" t="s">
-        <v>280</v>
-      </c>
-      <c r="G43" t="s">
-        <v>279</v>
-      </c>
-      <c r="H43" t="s">
-        <v>244</v>
-      </c>
-      <c r="I43" t="s">
-        <v>188</v>
-      </c>
-      <c r="K43" t="s">
-        <v>185</v>
-      </c>
-      <c r="L43" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
@@ -3102,34 +3108,34 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>187</v>
+      </c>
+      <c r="E44" t="s">
+        <v>188</v>
+      </c>
+      <c r="F44" t="s">
+        <v>280</v>
+      </c>
+      <c r="G44" t="s">
+        <v>279</v>
+      </c>
+      <c r="H44" t="s">
+        <v>242</v>
+      </c>
+      <c r="I44" t="s">
+        <v>192</v>
+      </c>
+      <c r="K44" t="s">
         <v>189</v>
       </c>
-      <c r="E44" t="s">
+      <c r="L44" t="s">
         <v>190</v>
-      </c>
-      <c r="F44" t="s">
-        <v>282</v>
-      </c>
-      <c r="G44" t="s">
-        <v>281</v>
-      </c>
-      <c r="H44" t="s">
-        <v>244</v>
-      </c>
-      <c r="I44" t="s">
-        <v>194</v>
-      </c>
-      <c r="K44" t="s">
-        <v>191</v>
-      </c>
-      <c r="L44" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
@@ -3137,37 +3143,37 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
+        <v>193</v>
+      </c>
+      <c r="E45" t="s">
+        <v>194</v>
+      </c>
+      <c r="F45" t="s">
+        <v>282</v>
+      </c>
+      <c r="G45" t="s">
+        <v>281</v>
+      </c>
+      <c r="H45" t="s">
+        <v>242</v>
+      </c>
+      <c r="I45" t="s">
+        <v>199</v>
+      </c>
+      <c r="K45" t="s">
         <v>195</v>
       </c>
-      <c r="E45" t="s">
+      <c r="L45" t="s">
         <v>196</v>
       </c>
-      <c r="F45" t="s">
-        <v>284</v>
-      </c>
-      <c r="G45" t="s">
-        <v>283</v>
-      </c>
-      <c r="H45" t="s">
-        <v>244</v>
-      </c>
-      <c r="I45" t="s">
-        <v>201</v>
-      </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
         <v>197</v>
-      </c>
-      <c r="L45" t="s">
-        <v>198</v>
-      </c>
-      <c r="M45" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -3175,37 +3181,37 @@
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" t="s">
+        <v>282</v>
+      </c>
+      <c r="G46" t="s">
+        <v>283</v>
+      </c>
+      <c r="H46" t="s">
+        <v>242</v>
+      </c>
+      <c r="I46" t="s">
+        <v>206</v>
+      </c>
+      <c r="K46" t="s">
         <v>202</v>
       </c>
-      <c r="E46" t="s">
+      <c r="L46" t="s">
         <v>203</v>
       </c>
-      <c r="F46" t="s">
-        <v>284</v>
-      </c>
-      <c r="G46" t="s">
-        <v>285</v>
-      </c>
-      <c r="H46" t="s">
-        <v>244</v>
-      </c>
-      <c r="I46" t="s">
-        <v>208</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="M46" t="s">
         <v>204</v>
-      </c>
-      <c r="L46" t="s">
-        <v>205</v>
-      </c>
-      <c r="M46" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
@@ -3213,37 +3219,37 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47" t="s">
+        <v>207</v>
+      </c>
+      <c r="E47" t="s">
+        <v>208</v>
+      </c>
+      <c r="F47" t="s">
+        <v>282</v>
+      </c>
+      <c r="G47" t="s">
+        <v>284</v>
+      </c>
+      <c r="H47" t="s">
+        <v>242</v>
+      </c>
+      <c r="I47" t="s">
+        <v>213</v>
+      </c>
+      <c r="K47" t="s">
         <v>209</v>
       </c>
-      <c r="E47" t="s">
+      <c r="L47" t="s">
         <v>210</v>
       </c>
-      <c r="F47" t="s">
-        <v>284</v>
-      </c>
-      <c r="G47" t="s">
-        <v>286</v>
-      </c>
-      <c r="H47" t="s">
-        <v>244</v>
-      </c>
-      <c r="I47" t="s">
-        <v>215</v>
-      </c>
-      <c r="K47" t="s">
+      <c r="M47" t="s">
         <v>211</v>
-      </c>
-      <c r="L47" t="s">
-        <v>212</v>
-      </c>
-      <c r="M47" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
@@ -3251,37 +3257,37 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
+        <v>214</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F48" t="s">
+        <v>282</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H48" t="s">
+        <v>242</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K48" t="s">
+        <v>215</v>
+      </c>
+      <c r="L48" t="s">
         <v>216</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="F48" t="s">
-        <v>284</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H48" t="s">
-        <v>244</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="M48" t="s">
         <v>217</v>
-      </c>
-      <c r="L48" t="s">
-        <v>218</v>
-      </c>
-      <c r="M48" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
@@ -3289,40 +3295,40 @@
         <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
+        <v>219</v>
+      </c>
+      <c r="E49" t="s">
+        <v>220</v>
+      </c>
+      <c r="F49" t="s">
+        <v>285</v>
+      </c>
+      <c r="G49" t="s">
+        <v>226</v>
+      </c>
+      <c r="H49" t="s">
+        <v>242</v>
+      </c>
+      <c r="I49" t="s">
+        <v>224</v>
+      </c>
+      <c r="K49" t="s">
         <v>221</v>
       </c>
-      <c r="E49" t="s">
+      <c r="L49" t="s">
         <v>222</v>
       </c>
-      <c r="F49" t="s">
-        <v>287</v>
-      </c>
-      <c r="G49" t="s">
-        <v>228</v>
-      </c>
-      <c r="H49" t="s">
-        <v>244</v>
-      </c>
-      <c r="I49" t="s">
-        <v>226</v>
-      </c>
-      <c r="K49" t="s">
+      <c r="M49" t="s">
         <v>223</v>
       </c>
-      <c r="L49" t="s">
-        <v>224</v>
-      </c>
-      <c r="M49" t="s">
+      <c r="P49" t="s">
         <v>225</v>
-      </c>
-      <c r="P49" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
@@ -3330,34 +3336,34 @@
         <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" t="s">
+        <v>285</v>
+      </c>
+      <c r="G50" t="s">
+        <v>286</v>
+      </c>
+      <c r="H50" t="s">
+        <v>242</v>
+      </c>
+      <c r="I50" t="s">
+        <v>232</v>
+      </c>
+      <c r="K50" t="s">
         <v>229</v>
       </c>
-      <c r="E50" t="s">
+      <c r="L50" t="s">
         <v>230</v>
-      </c>
-      <c r="F50" t="s">
-        <v>287</v>
-      </c>
-      <c r="G50" t="s">
-        <v>288</v>
-      </c>
-      <c r="H50" t="s">
-        <v>244</v>
-      </c>
-      <c r="I50" t="s">
-        <v>234</v>
-      </c>
-      <c r="K50" t="s">
-        <v>231</v>
-      </c>
-      <c r="L50" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
@@ -3365,37 +3371,37 @@
         <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E51" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F51" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G51" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H51" t="s">
         <v>21</v>
       </c>
       <c r="I51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K51" t="s">
+        <v>235</v>
+      </c>
+      <c r="L51" t="s">
+        <v>236</v>
+      </c>
+      <c r="M51" t="s">
         <v>237</v>
-      </c>
-      <c r="L51" t="s">
-        <v>238</v>
-      </c>
-      <c r="M51" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>